<commit_message>
14 elevators scripts added
latest elevators
</commit_message>
<xml_diff>
--- a/src/com/data/Test Cases Elc.xlsx
+++ b/src/com/data/Test Cases Elc.xlsx
@@ -537,25 +537,7 @@
     <t>1yes</t>
   </si>
   <si>
-    <t>Field Sign Inspection</t>
-  </si>
-  <si>
     <t>ElFieldSignInspectionTest</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Electrical </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Field Sign Inspection</t>
-    </r>
   </si>
   <si>
     <t>2yes</t>
@@ -679,6 +661,24 @@
   </si>
   <si>
     <t>Emergency Lighting (LL 16/84)</t>
+  </si>
+  <si>
+    <t>Field Sign</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Electrical </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Field Sign</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>3</v>
@@ -2640,7 +2640,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>3</v>
@@ -2648,7 +2648,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="35" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>3</v>
@@ -2656,7 +2656,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>3</v>
@@ -2677,9 +2677,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AF1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AP36" sqref="AP36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="15"/>
@@ -3137,7 +3137,7 @@
     </row>
     <row r="10" spans="1:53" s="15" customFormat="1" ht="12.75">
       <c r="A10" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
@@ -3164,10 +3164,10 @@
         <v>5</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G11" s="37" t="s">
         <v>6</v>
@@ -3316,7 +3316,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="C12" s="36" t="s">
         <v>25</v>
@@ -3325,10 +3325,10 @@
         <v>18</v>
       </c>
       <c r="E12" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G12" s="33" t="s">
         <v>16</v>
@@ -3367,7 +3367,7 @@
         <v>3</v>
       </c>
       <c r="W12" s="33" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="X12" s="38" t="s">
         <v>8</v>
@@ -3405,7 +3405,7 @@
     <row r="13" spans="1:53" s="31" customFormat="1"/>
     <row r="14" spans="1:53" s="15" customFormat="1" ht="12.75">
       <c r="A14" s="35" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -3432,10 +3432,10 @@
         <v>5</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F15" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G15" s="37" t="s">
         <v>6</v>
@@ -3584,7 +3584,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C16" s="36" t="s">
         <v>25</v>
@@ -3593,10 +3593,10 @@
         <v>18</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J16" s="33" t="s">
         <v>20</v>
@@ -3620,7 +3620,7 @@
         <v>132</v>
       </c>
       <c r="S16" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="U16" s="33" t="s">
         <v>3</v>
@@ -3667,7 +3667,7 @@
     <row r="17" spans="1:55" s="31" customFormat="1"/>
     <row r="18" spans="1:55" s="15" customFormat="1" ht="12.75">
       <c r="A18" s="35" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
@@ -3694,10 +3694,10 @@
         <v>5</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F19" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G19" s="37" t="s">
         <v>6</v>
@@ -3846,7 +3846,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C20" s="36" t="s">
         <v>25</v>
@@ -3855,10 +3855,10 @@
         <v>18</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F20" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J20" s="33" t="s">
         <v>20</v>
@@ -3882,13 +3882,13 @@
         <v>132</v>
       </c>
       <c r="S20" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="U20" s="33" t="s">
         <v>3</v>
       </c>
       <c r="W20" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X20" s="38" t="s">
         <v>8</v>
@@ -3956,10 +3956,10 @@
         <v>5</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F23" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G23" s="18" t="s">
         <v>6</v>
@@ -4117,10 +4117,10 @@
         <v>18</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>16</v>
@@ -4223,10 +4223,10 @@
         <v>5</v>
       </c>
       <c r="E27" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F27" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G27" s="18" t="s">
         <v>6</v>
@@ -4375,7 +4375,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C28" s="22" t="s">
         <v>25</v>
@@ -4384,10 +4384,10 @@
         <v>18</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>16</v>
@@ -4426,7 +4426,7 @@
         <v>3</v>
       </c>
       <c r="W28" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X28" s="17" t="s">
         <v>8</v>
@@ -4488,10 +4488,10 @@
         <v>5</v>
       </c>
       <c r="E31" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F31" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G31" s="37" t="s">
         <v>6</v>
@@ -4509,7 +4509,7 @@
         <v>21</v>
       </c>
       <c r="L31" s="37" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M31" s="34" t="s">
         <v>32</v>
@@ -4646,7 +4646,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C32" s="36" t="s">
         <v>25</v>
@@ -4655,10 +4655,10 @@
         <v>18</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G32" s="33" t="s">
         <v>16</v>
@@ -4676,7 +4676,7 @@
         <v>22</v>
       </c>
       <c r="L32" s="36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M32" s="33" t="s">
         <v>25</v>
@@ -4700,7 +4700,7 @@
         <v>3</v>
       </c>
       <c r="W32" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X32" s="38" t="s">
         <v>8</v>
@@ -4757,7 +4757,7 @@
         <v>59</v>
       </c>
       <c r="AP32" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AQ32" s="38" t="s">
         <v>8</v>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="34" spans="1:55" s="15" customFormat="1" ht="12" customHeight="1">
       <c r="A34" s="35" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
@@ -4805,10 +4805,10 @@
         <v>5</v>
       </c>
       <c r="E35" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F35" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G35" s="37" t="s">
         <v>6</v>
@@ -4826,7 +4826,7 @@
         <v>21</v>
       </c>
       <c r="L35" s="37" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M35" s="34" t="s">
         <v>32</v>
@@ -4963,7 +4963,7 @@
         <v>3</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C36" s="36" t="s">
         <v>25</v>
@@ -4972,10 +4972,10 @@
         <v>18</v>
       </c>
       <c r="E36" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F36" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G36" s="33" t="s">
         <v>16</v>
@@ -4993,7 +4993,7 @@
         <v>22</v>
       </c>
       <c r="L36" s="36" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="M36" s="33" t="s">
         <v>25</v>
@@ -5017,7 +5017,7 @@
         <v>3</v>
       </c>
       <c r="W36" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X36" s="38" t="s">
         <v>8</v>
@@ -5074,7 +5074,7 @@
         <v>59</v>
       </c>
       <c r="AP36" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AQ36" s="38" t="s">
         <v>8</v>
@@ -5123,10 +5123,10 @@
         <v>5</v>
       </c>
       <c r="E39" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F39" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G39" s="18" t="s">
         <v>6</v>
@@ -5144,7 +5144,7 @@
         <v>21</v>
       </c>
       <c r="L39" s="37" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M39" s="12" t="s">
         <v>32</v>
@@ -5290,10 +5290,10 @@
         <v>18</v>
       </c>
       <c r="E40" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F40" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G40" s="11" t="s">
         <v>16</v>
@@ -5311,7 +5311,7 @@
         <v>22</v>
       </c>
       <c r="L40" s="36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M40" s="11" t="s">
         <v>25</v>
@@ -5335,7 +5335,7 @@
         <v>3</v>
       </c>
       <c r="W40" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X40" s="17" t="s">
         <v>8</v>
@@ -5344,7 +5344,7 @@
         <v>3</v>
       </c>
       <c r="Z40" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AA40" s="11" t="s">
         <v>3</v>
@@ -5428,10 +5428,10 @@
         <v>5</v>
       </c>
       <c r="E43" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F43" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G43" s="37" t="s">
         <v>6</v>
@@ -5580,7 +5580,7 @@
         <v>3</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C44" s="36" t="s">
         <v>25</v>
@@ -5589,10 +5589,10 @@
         <v>18</v>
       </c>
       <c r="E44" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F44" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G44" s="33" t="s">
         <v>16</v>
@@ -5634,7 +5634,7 @@
         <v>3</v>
       </c>
       <c r="W44" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X44" s="38" t="s">
         <v>8</v>
@@ -5745,10 +5745,10 @@
         <v>5</v>
       </c>
       <c r="E47" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F47" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G47" s="37" t="s">
         <v>6</v>
@@ -5906,10 +5906,10 @@
         <v>18</v>
       </c>
       <c r="E48" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F48" s="33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G48" s="33" t="s">
         <v>16</v>
@@ -6016,10 +6016,10 @@
         <v>5</v>
       </c>
       <c r="E51" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F51" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G51" s="37" t="s">
         <v>6</v>
@@ -6177,10 +6177,10 @@
         <v>18</v>
       </c>
       <c r="E52" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F52" s="33" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G52" s="33" t="s">
         <v>16</v>
@@ -6287,10 +6287,10 @@
         <v>5</v>
       </c>
       <c r="E55" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F55" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G55" s="37" t="s">
         <v>6</v>
@@ -6308,7 +6308,7 @@
         <v>21</v>
       </c>
       <c r="L55" s="37" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M55" s="34" t="s">
         <v>32</v>
@@ -6454,10 +6454,10 @@
         <v>18</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F56" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G56" s="33" t="s">
         <v>16</v>
@@ -6475,7 +6475,7 @@
         <v>22</v>
       </c>
       <c r="L56" s="36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M56" s="33" t="s">
         <v>25</v>
@@ -6499,7 +6499,7 @@
         <v>3</v>
       </c>
       <c r="W56" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X56" s="38" t="s">
         <v>8</v>
@@ -6556,7 +6556,7 @@
         <v>59</v>
       </c>
       <c r="AP56" s="33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AQ56" s="38" t="s">
         <v>8</v>
@@ -6605,10 +6605,10 @@
         <v>5</v>
       </c>
       <c r="E59" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F59" s="39" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G59" s="37" t="s">
         <v>6</v>
@@ -6626,7 +6626,7 @@
         <v>21</v>
       </c>
       <c r="L59" s="37" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="M59" s="34" t="s">
         <v>32</v>
@@ -6772,10 +6772,10 @@
         <v>18</v>
       </c>
       <c r="E60" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F60" s="33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G60" s="33" t="s">
         <v>16</v>
@@ -6793,7 +6793,7 @@
         <v>22</v>
       </c>
       <c r="L60" s="36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M60" s="33" t="s">
         <v>25</v>
@@ -6817,7 +6817,7 @@
         <v>3</v>
       </c>
       <c r="W60" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="X60" s="38" t="s">
         <v>8</v>
@@ -6874,7 +6874,7 @@
         <v>59</v>
       </c>
       <c r="AP60" s="33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AQ60" s="38" t="s">
         <v>8</v>
@@ -7024,7 +7024,7 @@
         <v>5</v>
       </c>
       <c r="E65" s="37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F65" s="19" t="s">
         <v>34</v>
@@ -7185,7 +7185,7 @@
         <v>18</v>
       </c>
       <c r="E66" s="33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L66" s="11" t="s">
         <v>79</v>

</xml_diff>